<commit_message>
final commit for this project. Project terminates here (for now). Not complete
</commit_message>
<xml_diff>
--- a/VisionModel/one_model/output/predicted_trajectories_DartsCombined.xlsx
+++ b/VisionModel/one_model/output/predicted_trajectories_DartsCombined.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>frame</t>
+          <t>time</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -460,643 +460,629 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1461.03</v>
+        <v>3361.16</v>
       </c>
       <c r="C2" t="n">
-        <v>94.75</v>
+        <v>161.07</v>
       </c>
       <c r="D2" t="n">
-        <v>2854.2</v>
+        <v>3823.24</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="B3" t="n">
-        <v>2363.36</v>
+        <v>4186.059999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>156.21</v>
+        <v>159.87</v>
       </c>
       <c r="D3" t="n">
-        <v>3291.03</v>
+        <v>4237.17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="B4" t="n">
-        <v>3361.16</v>
+        <v>4931.58</v>
       </c>
       <c r="C4" t="n">
-        <v>161.07</v>
+        <v>187.57</v>
       </c>
       <c r="D4" t="n">
-        <v>3823.24</v>
+        <v>4619.700000000001</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="B5" t="n">
-        <v>4186.059999999999</v>
+        <v>5584.19</v>
       </c>
       <c r="C5" t="n">
-        <v>159.87</v>
+        <v>207.51</v>
       </c>
       <c r="D5" t="n">
-        <v>4237.17</v>
+        <v>4940.68</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="B6" t="n">
-        <v>4931.58</v>
+        <v>6107.5</v>
       </c>
       <c r="C6" t="n">
-        <v>187.57</v>
+        <v>225.18</v>
       </c>
       <c r="D6" t="n">
-        <v>4619.700000000001</v>
+        <v>5180.700000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="B7" t="n">
-        <v>5584.19</v>
+        <v>6575.90673828125</v>
       </c>
       <c r="C7" t="n">
-        <v>207.51</v>
+        <v>236.2182312011719</v>
       </c>
       <c r="D7" t="n">
-        <v>4940.68</v>
+        <v>5403.08056640625</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="B8" t="n">
-        <v>6072.39990234375</v>
+        <v>6943.58837890625</v>
       </c>
       <c r="C8" t="n">
-        <v>218.9627838134766</v>
+        <v>249.4012145996094</v>
       </c>
       <c r="D8" t="n">
-        <v>5188.2578125</v>
+        <v>5598.44287109375</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="B9" t="n">
-        <v>6585.94189453125</v>
+        <v>7354.48193359375</v>
       </c>
       <c r="C9" t="n">
-        <v>226.6117553710938</v>
+        <v>267.7780151367188</v>
       </c>
       <c r="D9" t="n">
-        <v>5471.86767578125</v>
+        <v>5918.787109375</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="B10" t="n">
-        <v>6881.35107421875</v>
+        <v>7820.8212890625</v>
       </c>
       <c r="C10" t="n">
-        <v>233.1102600097656</v>
+        <v>274.03369140625</v>
       </c>
       <c r="D10" t="n">
-        <v>5672.57861328125</v>
+        <v>6098.466796875</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>0.3</v>
       </c>
       <c r="B11" t="n">
-        <v>7380.22119140625</v>
+        <v>8161.99462890625</v>
       </c>
       <c r="C11" t="n">
-        <v>247.5807037353516</v>
+        <v>294.5572814941406</v>
       </c>
       <c r="D11" t="n">
-        <v>5619.322265625</v>
+        <v>6165.677734375</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="B12" t="n">
-        <v>7768.1640625</v>
+        <v>8260.9755859375</v>
       </c>
       <c r="C12" t="n">
-        <v>258.0289916992188</v>
+        <v>300.0196533203125</v>
       </c>
       <c r="D12" t="n">
-        <v>6031.0263671875</v>
+        <v>6194.69482421875</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>11</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="B13" t="n">
-        <v>8141.83837890625</v>
+        <v>8648.302734375</v>
       </c>
       <c r="C13" t="n">
-        <v>285.4479064941406</v>
+        <v>316.169677734375</v>
       </c>
       <c r="D13" t="n">
-        <v>6243.0439453125</v>
+        <v>6057.314453125</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>12</v>
+        <v>0.4</v>
       </c>
       <c r="B14" t="n">
-        <v>8370.5380859375</v>
+        <v>8980.2841796875</v>
       </c>
       <c r="C14" t="n">
-        <v>277.2198486328125</v>
+        <v>310.091796875</v>
       </c>
       <c r="D14" t="n">
-        <v>6166.21142578125</v>
+        <v>5855.31982421875</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>13</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="B15" t="n">
-        <v>8546.5341796875</v>
+        <v>9310.3203125</v>
       </c>
       <c r="C15" t="n">
-        <v>293.3254699707031</v>
+        <v>328.6161499023438</v>
       </c>
       <c r="D15" t="n">
-        <v>6558.919921875</v>
+        <v>5954.09033203125</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>14</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="B16" t="n">
-        <v>9119.7275390625</v>
+        <v>9640.638671875</v>
       </c>
       <c r="C16" t="n">
-        <v>319.7737121582031</v>
+        <v>333.1732177734375</v>
       </c>
       <c r="D16" t="n">
-        <v>6662.53271484375</v>
+        <v>5976.60302734375</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>15</v>
+        <v>0.5</v>
       </c>
       <c r="B17" t="n">
-        <v>9327.5390625</v>
+        <v>9579.0205078125</v>
       </c>
       <c r="C17" t="n">
-        <v>339.7258911132812</v>
+        <v>347.687744140625</v>
       </c>
       <c r="D17" t="n">
-        <v>6805.7314453125</v>
+        <v>6012.90576171875</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>16</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="B18" t="n">
-        <v>9588.2734375</v>
+        <v>9763.2744140625</v>
       </c>
       <c r="C18" t="n">
-        <v>323.6983337402344</v>
+        <v>369.9434204101562</v>
       </c>
       <c r="D18" t="n">
-        <v>6850.68359375</v>
+        <v>5961.96875</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>17</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="B19" t="n">
-        <v>9861.4970703125</v>
+        <v>10485.654296875</v>
       </c>
       <c r="C19" t="n">
-        <v>363.6722717285156</v>
+        <v>371.8629150390625</v>
       </c>
       <c r="D19" t="n">
-        <v>6901.97265625</v>
+        <v>5948.7041015625</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>18</v>
+        <v>0.6</v>
       </c>
       <c r="B20" t="n">
-        <v>10080.048828125</v>
+        <v>10408.322265625</v>
       </c>
       <c r="C20" t="n">
-        <v>374.9489440917969</v>
+        <v>395.4696655273438</v>
       </c>
       <c r="D20" t="n">
-        <v>6968.6513671875</v>
+        <v>6054.97900390625</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>19</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="B21" t="n">
-        <v>10194.8701171875</v>
+        <v>10924.951171875</v>
       </c>
       <c r="C21" t="n">
-        <v>401.7854919433594</v>
+        <v>404.6325378417969</v>
       </c>
       <c r="D21" t="n">
-        <v>6989.18701171875</v>
+        <v>6056.05517578125</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>20</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>10306.9169921875</v>
+        <v>10754.6533203125</v>
       </c>
       <c r="C22" t="n">
-        <v>383.0676879882812</v>
+        <v>432.5109252929688</v>
       </c>
       <c r="D22" t="n">
-        <v>7034.6552734375</v>
+        <v>6068.1259765625</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>21</v>
+        <v>0.7</v>
       </c>
       <c r="B23" t="n">
-        <v>10666.7001953125</v>
+        <v>10950.1708984375</v>
       </c>
       <c r="C23" t="n">
-        <v>391.6213989257812</v>
+        <v>429.2830505371094</v>
       </c>
       <c r="D23" t="n">
-        <v>7024.60205078125</v>
+        <v>6007.95654296875</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>22</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="B24" t="n">
-        <v>10873.794921875</v>
+        <v>11347.779296875</v>
       </c>
       <c r="C24" t="n">
-        <v>391.2892150878906</v>
+        <v>444.1619873046875</v>
       </c>
       <c r="D24" t="n">
-        <v>6926.990234375</v>
+        <v>6088.14501953125</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>23</v>
+        <v>0.7666666666666666</v>
       </c>
       <c r="B25" t="n">
-        <v>11005.876953125</v>
+        <v>11721.0654296875</v>
       </c>
       <c r="C25" t="n">
-        <v>409.4625549316406</v>
+        <v>438.49658203125</v>
       </c>
       <c r="D25" t="n">
-        <v>6847.1259765625</v>
+        <v>6001.56884765625</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>24</v>
+        <v>0.8</v>
       </c>
       <c r="B26" t="n">
-        <v>11023.9501953125</v>
+        <v>12283.880859375</v>
       </c>
       <c r="C26" t="n">
-        <v>441.8912048339844</v>
+        <v>479.1244812011719</v>
       </c>
       <c r="D26" t="n">
-        <v>6878.126953125</v>
+        <v>6028.923828125</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>25</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="B27" t="n">
-        <v>11362.099609375</v>
+        <v>12548.7451171875</v>
       </c>
       <c r="C27" t="n">
-        <v>468.6517944335938</v>
+        <v>468.9779357910156</v>
       </c>
       <c r="D27" t="n">
-        <v>6837.1875</v>
+        <v>5860.23388671875</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>26</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="B28" t="n">
-        <v>11450.60546875</v>
+        <v>12832.2314453125</v>
       </c>
       <c r="C28" t="n">
-        <v>466.0384216308594</v>
+        <v>490.4096984863281</v>
       </c>
       <c r="D28" t="n">
-        <v>6742.35888671875</v>
+        <v>5889.4375</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>27</v>
+        <v>0.9</v>
       </c>
       <c r="B29" t="n">
-        <v>11844.4404296875</v>
+        <v>12980.322265625</v>
       </c>
       <c r="C29" t="n">
-        <v>447.7886352539062</v>
+        <v>488.933837890625</v>
       </c>
       <c r="D29" t="n">
-        <v>6761.57275390625</v>
+        <v>5626.94384765625</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>28</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="B30" t="n">
-        <v>11845.076171875</v>
+        <v>13030.3251953125</v>
       </c>
       <c r="C30" t="n">
-        <v>412.0097961425781</v>
+        <v>515.1332397460938</v>
       </c>
       <c r="D30" t="n">
-        <v>6555.57421875</v>
+        <v>5215.01953125</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>29</v>
+        <v>0.9666666666666667</v>
       </c>
       <c r="B31" t="n">
-        <v>12218.1494140625</v>
+        <v>13698.9150390625</v>
       </c>
       <c r="C31" t="n">
-        <v>493.9302978515625</v>
+        <v>521.6781005859375</v>
       </c>
       <c r="D31" t="n">
-        <v>6387.2080078125</v>
+        <v>5504.654296875</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>12447.064453125</v>
+        <v>13692.474609375</v>
       </c>
       <c r="C32" t="n">
-        <v>495.3658142089844</v>
+        <v>560.6834716796875</v>
       </c>
       <c r="D32" t="n">
-        <v>6436.25439453125</v>
+        <v>5466.75341796875</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>31</v>
+        <v>1.033333333333333</v>
       </c>
       <c r="B33" t="n">
-        <v>12358.404296875</v>
+        <v>13578.8896484375</v>
       </c>
       <c r="C33" t="n">
-        <v>531.2738037109375</v>
+        <v>559.1596069335938</v>
       </c>
       <c r="D33" t="n">
-        <v>6241.01025390625</v>
+        <v>4951.1943359375</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>32</v>
+        <v>1.066666666666667</v>
       </c>
       <c r="B34" t="n">
-        <v>12657.3564453125</v>
+        <v>14050.3671875</v>
       </c>
       <c r="C34" t="n">
-        <v>545.052978515625</v>
+        <v>575.5615234375</v>
       </c>
       <c r="D34" t="n">
-        <v>6038.05712890625</v>
+        <v>4701.361328125</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>33</v>
+        <v>1.1</v>
       </c>
       <c r="B35" t="n">
-        <v>12807.3271484375</v>
+        <v>14201.75</v>
       </c>
       <c r="C35" t="n">
-        <v>526.2437133789062</v>
+        <v>558.1874389648438</v>
       </c>
       <c r="D35" t="n">
-        <v>5939.32080078125</v>
+        <v>4488.10009765625</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>34</v>
+        <v>1.133333333333333</v>
       </c>
       <c r="B36" t="n">
-        <v>13026.5634765625</v>
+        <v>14715.02734375</v>
       </c>
       <c r="C36" t="n">
-        <v>546.2344360351562</v>
+        <v>600.772705078125</v>
       </c>
       <c r="D36" t="n">
-        <v>6067.18798828125</v>
+        <v>4631.6962890625</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>35</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="B37" t="n">
-        <v>13011.1279296875</v>
+        <v>14672.5234375</v>
       </c>
       <c r="C37" t="n">
-        <v>553.3564453125</v>
+        <v>601.9946899414062</v>
       </c>
       <c r="D37" t="n">
-        <v>5435.47900390625</v>
+        <v>4328.28125</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>36</v>
+        <v>1.2</v>
       </c>
       <c r="B38" t="n">
-        <v>13230.810546875</v>
+        <v>14801.24609375</v>
       </c>
       <c r="C38" t="n">
-        <v>565.3256225585938</v>
+        <v>616.7559204101562</v>
       </c>
       <c r="D38" t="n">
-        <v>5402.396484375</v>
+        <v>4486.13525390625</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>37</v>
+        <v>1.233333333333333</v>
       </c>
       <c r="B39" t="n">
-        <v>13346.158203125</v>
+        <v>15043.8623046875</v>
       </c>
       <c r="C39" t="n">
-        <v>551.3818969726562</v>
+        <v>634.1895141601562</v>
       </c>
       <c r="D39" t="n">
-        <v>5217.765625</v>
+        <v>3742.700439453125</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>38</v>
+        <v>1.266666666666667</v>
       </c>
       <c r="B40" t="n">
-        <v>13504.546875</v>
+        <v>15052.2470703125</v>
       </c>
       <c r="C40" t="n">
-        <v>600.4367065429688</v>
+        <v>664.1375732421875</v>
       </c>
       <c r="D40" t="n">
-        <v>5406.74365234375</v>
+        <v>3880.383056640625</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>39</v>
+        <v>1.3</v>
       </c>
       <c r="B41" t="n">
-        <v>13656.2587890625</v>
+        <v>15351.3115234375</v>
       </c>
       <c r="C41" t="n">
-        <v>596.955078125</v>
+        <v>654.01220703125</v>
       </c>
       <c r="D41" t="n">
-        <v>4768.66748046875</v>
+        <v>3647.98583984375</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>40</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="B42" t="n">
-        <v>13847.990234375</v>
+        <v>15331.12890625</v>
       </c>
       <c r="C42" t="n">
-        <v>616.1541748046875</v>
+        <v>676.2843627929688</v>
       </c>
       <c r="D42" t="n">
-        <v>5178.66455078125</v>
+        <v>3557.614990234375</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>41</v>
+        <v>1.366666666666667</v>
       </c>
       <c r="B43" t="n">
-        <v>13718.9072265625</v>
+        <v>15523.6337890625</v>
       </c>
       <c r="C43" t="n">
-        <v>602.2060546875</v>
+        <v>696.7689819335938</v>
       </c>
       <c r="D43" t="n">
-        <v>4590.607421875</v>
+        <v>3703.0693359375</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>42</v>
+        <v>1.4</v>
       </c>
       <c r="B44" t="n">
-        <v>13883.3564453125</v>
+        <v>15650.4189453125</v>
       </c>
       <c r="C44" t="n">
-        <v>616.4960327148438</v>
+        <v>706.6704711914062</v>
       </c>
       <c r="D44" t="n">
-        <v>4439.66259765625</v>
+        <v>3943.83837890625</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>43</v>
+        <v>1.433333333333333</v>
       </c>
       <c r="B45" t="n">
-        <v>13934.408203125</v>
+        <v>15672.220703125</v>
       </c>
       <c r="C45" t="n">
-        <v>645.7083129882812</v>
+        <v>721.937744140625</v>
       </c>
       <c r="D45" t="n">
-        <v>4185.017578125</v>
+        <v>4368.83349609375</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>44</v>
+        <v>1.466666666666667</v>
       </c>
       <c r="B46" t="n">
-        <v>14145.32421875</v>
+        <v>15970.0244140625</v>
       </c>
       <c r="C46" t="n">
-        <v>670.589599609375</v>
+        <v>748.906494140625</v>
       </c>
       <c r="D46" t="n">
-        <v>4098.13427734375</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="n">
-        <v>14227.6708984375</v>
-      </c>
-      <c r="C47" t="n">
-        <v>646.668212890625</v>
-      </c>
-      <c r="D47" t="n">
-        <v>3869.988525390625</v>
+        <v>3908.42724609375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>